<commit_message>
Updated Flask app with latest changes
</commit_message>
<xml_diff>
--- a/data/details.xlsx
+++ b/data/details.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
+    <sheet r:id="rId3" sheetId="3" name="Sheet3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -33,85 +33,85 @@
     <t>Section 125, Code of Criminal Procedure, 1973</t>
   </si>
   <si>
+    <t>The court is likely to rule in favor of the wife and child. The husband may be ordered to pay a fixed monthly maintenance amount, considering his financial stability. Additionally, the court might warn that failure to comply could lead to salary garnishment or even imprisonment.</t>
+  </si>
+  <si>
     <t>I want to file for divorce because my husband has been physically and mentally abusive. I have medical reports and witness testimonies to prove my claims.</t>
   </si>
   <si>
     <t>Section 13(1)(ia), Hindu Marriage Act, 1955</t>
   </si>
   <si>
+    <t>The court is likely to grant the divorce on grounds of cruelty. The judgment might include an order for alimony or financial support to the wife.</t>
+  </si>
+  <si>
     <t>I want to annul my marriage because I recently found out that my spouse was already married at the time of our wedding.</t>
   </si>
   <si>
     <t>Section 24, Special Marriage Act, 1954</t>
   </si>
   <si>
+    <t>The court will likely declare the marriage null and void. The judgment may also include legal consequences for the spouse under bigamy laws.</t>
+  </si>
+  <si>
     <t>I want to file a petition because my ex-husband is refusing to let me visit my child, even though the court granted me visitation rights.</t>
   </si>
   <si>
     <t>Section 26, Hindu Marriage Act, 1955</t>
   </si>
   <si>
+    <t>The court will reinforce the mother's visitation rights and may issue a warning to the father. If non-compliance continues, the court might impose penalties or modify custody arrangements.</t>
+  </si>
+  <si>
     <t>I want to challenge my husband's decision to give me triple talaq. He sent me a message declaring instant divorce.</t>
   </si>
   <si>
     <t>Muslim Women (Protection of Rights on Marriage) Act, 2019</t>
   </si>
   <si>
+    <t>The court will declare the triple talaq invalid. The judgment may include financial support for the wife and legal action against the husband for violating the law.</t>
+  </si>
+  <si>
     <t>I want to claim my share in my father’s ancestral property. My brothers are refusing to give me my rightful inheritance.</t>
   </si>
   <si>
     <t>Section 6, Hindu Succession Act, 1956</t>
   </si>
   <si>
+    <t>The court will recognize the daughter's equal rights in ancestral property under the amended Hindu Succession Act. The judgment is likely to order an equal partition of the property in her favor.</t>
+  </si>
+  <si>
     <t>I want to file for divorce because my husband has been unfaithful. I have evidence of his adulterous relationship.</t>
   </si>
   <si>
     <t>Section 13(1)(i), Hindu Marriage Act, 1955</t>
   </si>
   <si>
+    <t>The court will examine the evidence thoroughly. If the proof is found to be conclusive, the court may grant the divorce on grounds of adultery. However, if the evidence is weak, the case might be dismissed or redirected to mediation.</t>
+  </si>
+  <si>
     <t>I want to file a complaint under the Domestic Violence Act because I have suffered emotional and financial abuse from my husband and in-laws.</t>
   </si>
   <si>
     <t>Sections 12, 18, 19, Protection of Women from Domestic Violence Act, 2005</t>
   </si>
   <si>
+    <t>The court is likely to grant protection, residence rights, and financial support to the woman. A restraining order may be issued against the in-laws to prevent further abuse.</t>
+  </si>
+  <si>
     <t>I want to adopt a child, but legal authorities are delaying the process. I meet all eligibility criteria under adoption laws.</t>
   </si>
   <si>
     <t>Section 56, Juvenile Justice (Care and Protection of Children) Act, 2015</t>
   </si>
   <si>
+    <t>The court will order the authorities to expedite the adoption process, ensuring compliance with legal procedures while prioritizing the child’s welfare.</t>
+  </si>
+  <si>
     <t>I want to file for divorce because my husband abandoned me two years ago and has not contacted me since.</t>
   </si>
   <si>
     <t>Section 10(1)(ix), Indian Divorce Act, 1869</t>
-  </si>
-  <si>
-    <t>The court is likely to rule in favor of the wife and child. The husband may be ordered to pay a fixed monthly maintenance amount, considering his financial stability. Additionally, the court might warn that failure to comply could lead to salary garnishment or even imprisonment.</t>
-  </si>
-  <si>
-    <t>The court is likely to grant the divorce on grounds of cruelty. The judgment might include an order for alimony or financial support to the wife.</t>
-  </si>
-  <si>
-    <t>The court will likely declare the marriage null and void. The judgment may also include legal consequences for the spouse under bigamy laws.</t>
-  </si>
-  <si>
-    <t>The court will reinforce the mother's visitation rights and may issue a warning to the father. If non-compliance continues, the court might impose penalties or modify custody arrangements.</t>
-  </si>
-  <si>
-    <t>The court will declare the triple talaq invalid. The judgment may include financial support for the wife and legal action against the husband for violating the law.</t>
-  </si>
-  <si>
-    <t>The court will recognize the daughter's equal rights in ancestral property under the amended Hindu Succession Act. The judgment is likely to order an equal partition of the property in her favor.</t>
-  </si>
-  <si>
-    <t>The court will examine the evidence thoroughly. If the proof is found to be conclusive, the court may grant the divorce on grounds of adultery. However, if the evidence is weak, the case might be dismissed or redirected to mediation.</t>
-  </si>
-  <si>
-    <t>The court is likely to grant protection, residence rights, and financial support to the woman. A restraining order may be issued against the in-laws to prevent further abuse.</t>
-  </si>
-  <si>
-    <t>The court will order the authorities to expedite the adoption process, ensuring compliance with legal procedures while prioritizing the child’s welfare.</t>
   </si>
   <si>
     <t>The court is likely to grant the divorce on grounds of desertion. The judgment may be issued in the wife's favor, with possible financial compensation.</t>
@@ -120,8 +120,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,18 +133,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +153,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -166,20 +172,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <extLst>
     <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
@@ -192,10 +205,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -233,71 +246,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -325,7 +338,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -348,11 +361,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -361,13 +374,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -377,7 +390,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -386,7 +399,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -395,7 +408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -403,10 +416,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -471,141 +484,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="78.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="79.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="41.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="78.7192857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -615,7 +626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -623,14 +634,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -638,7 +649,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>